<commit_message>
Update Function For Detect Text in Terminal
</commit_message>
<xml_diff>
--- a/Excel/SimATM - SCIC0007 - ATM Processing.xlsx
+++ b/Excel/SimATM - SCIC0007 - ATM Processing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\ICONS\Excel\Trial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\ICONS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCD1382-A5C9-4284-A067-3F3249DD5BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6D1F7A-B6A3-403A-8F5F-421E5726FFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{5E7B8BF1-A296-4B05-868D-4DC65ED38144}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>RUN</t>
   </si>
@@ -478,7 +478,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,9 +576,6 @@
       <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
@@ -609,9 +606,6 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Update Get JNL and FM acc Number By Screen Text
</commit_message>
<xml_diff>
--- a/Excel/SimATM - SCIC0007 - ATM Processing.xlsx
+++ b/Excel/SimATM - SCIC0007 - ATM Processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\ICONS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6D1F7A-B6A3-403A-8F5F-421E5726FFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3439A7-3670-40C5-838E-74167CD5F7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{5E7B8BF1-A296-4B05-868D-4DC65ED38144}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>RUN</t>
   </si>
@@ -478,7 +478,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,6 +576,9 @@
       <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
@@ -606,6 +609,9 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>